<commit_message>
wrote some stuff down in the diary
</commit_message>
<xml_diff>
--- a/ResearchDiary/RelatedWorkTabelle.xlsx
+++ b/ResearchDiary/RelatedWorkTabelle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmaer\Documents\FH\Projects\MasterArbeit\mmt-masterarbeit-david-maerzendorfer\ResearchDiary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025D0DF6-EC98-44D3-B107-ADB6727023C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127D1751-6D4A-4295-80BA-D61D97391E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="164">
   <si>
     <t>Paper</t>
   </si>
@@ -408,13 +408,130 @@
   </si>
   <si>
     <t>Avatar Embodiment. Towards a Standardized Questionnaire</t>
+  </si>
+  <si>
+    <t>https://github.com/microsoft/Microsoft-Rocketbox</t>
+  </si>
+  <si>
+    <t>avatar lib by microsoft also has a paper on the avatar lib</t>
+  </si>
+  <si>
+    <t>MICROSOFT ROCKETBOX AVATAR LIBRARY</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?view_op=view_citation&amp;hl=en&amp;user=Fs0fyasAAAAJ&amp;citation_for_view=Fs0fyasAAAAJ:fPk4N6BV_jEC</t>
+  </si>
+  <si>
+    <t>markus paper on object orientated viewing of eG a house or other big sight. The thingy on when you want to see the back of the kölner dom. Phone based tho.</t>
+  </si>
+  <si>
+    <t>Markus Tatzgern, et. al.</t>
+  </si>
+  <si>
+    <t>exploring real world points of interest: Design and evaluation of object-centric exploration techniques for augmented reality</t>
+  </si>
+  <si>
+    <t>Voodoo dolls: seamless interaction at multiple scales in virtual environments</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/abs/10.1145/300523.300540</t>
+  </si>
+  <si>
+    <t>Jeffrey S. Pierce, et. Al.</t>
+  </si>
+  <si>
+    <t>viewing eG an exhibit in the palm of your hand and manipulating it. Kind of like a world in miniature, but is more for manipulating an object far away and its two handed. Pretty much like my world in miniature.</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/2212776.2212394</t>
+  </si>
+  <si>
+    <t>taking views/snapshots of objects in AR and switching between them!</t>
+  </si>
+  <si>
+    <t>Using augmented snapshots for viewpoint switching and manipulation in augmented reality</t>
+  </si>
+  <si>
+    <t>Mengu Sukan, et. Al.</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/261135.261141</t>
+  </si>
+  <si>
+    <t>basic paper on manipulation framework in VR, might be good for breaking down what kind of manipulation is important for viewpoints. eG we don’t care about scaling!</t>
+  </si>
+  <si>
+    <t>A framework and testbed for studying manipulation techniques for immersive VR</t>
+  </si>
+  <si>
+    <t>Ivan Poupyrev, et. Al.</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/3485279.3485296</t>
+  </si>
+  <si>
+    <t>Design and Empirical Evaluation of a Novel Near-field Interaction Metaphor on Distant Object Manipulation in VR</t>
+  </si>
+  <si>
+    <t>widget based translation, rotation and scaling for distant objects</t>
+  </si>
+  <si>
+    <t>Chia-Yang Lee, et al</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/3563657.3595985</t>
+  </si>
+  <si>
+    <t>Participation Patterns of Interactive Playful Museum Exhibits: Evaluating the Participant Journey Map through Situated Observations</t>
+  </si>
+  <si>
+    <t>study on what participants do/look at during museum visit, maybe interesting to bring across the use-case of my own study</t>
+  </si>
+  <si>
+    <t>Danica Mast et al</t>
+  </si>
+  <si>
+    <t>https://epgp.inflibnet.ac.in/epgpdata/uploads/epgp_content/S000829IC/P001546/M024848/ET/1510309259P15-M14-TypesofExhibitions-ET.pdf</t>
+  </si>
+  <si>
+    <t>some info on exhibits</t>
+  </si>
+  <si>
+    <t>Types of Exhibitions</t>
+  </si>
+  <si>
+    <t>https://www.icom-italia.org/wp-content/uploads/2018/02/ICOMItalia.KeyconceptsofMuseology.Pubblicazioni.2010.pdf</t>
+  </si>
+  <si>
+    <t>key concepts of museology</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/3411764.3445193</t>
+  </si>
+  <si>
+    <t>How to Evaluate Object Selection and Manipulation in VR? Guidelines from 20 Years of Studies</t>
+  </si>
+  <si>
+    <t>joanna bergström et al</t>
+  </si>
+  <si>
+    <t>Wall-based Space Manipulation Technique for Efficient Placement of Distant Objects in Augmented Reality</t>
+  </si>
+  <si>
+    <t>Hann joo chae et al</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/3242587.3242631</t>
+  </si>
+  <si>
+    <t>method for manipulating distant things in VR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -545,6 +662,36 @@
       <name val="Georgia"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16.5"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -597,7 +744,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -664,6 +811,21 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -814,8 +976,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F5384B4F-E58A-4FDF-9026-5EF3EE172CA3}" name="Tabelle2" displayName="Tabelle2" ref="A1:J40" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
-  <autoFilter ref="A1:J40" xr:uid="{622A20CF-99C6-4D06-B80E-EDF4CD2ACC21}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F5384B4F-E58A-4FDF-9026-5EF3EE172CA3}" name="Tabelle2" displayName="Tabelle2" ref="A1:J41" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+  <autoFilter ref="A1:J41" xr:uid="{622A20CF-99C6-4D06-B80E-EDF4CD2ACC21}"/>
   <tableColumns count="10">
     <tableColumn id="10" xr3:uid="{3982B8B8-D4C3-477E-982F-5AF76F683E58}" name="Authors" dataDxfId="33"/>
     <tableColumn id="1" xr3:uid="{EA04F39E-73D9-490A-863B-16A3A0920927}" name="Paper" dataDxfId="32"/>
@@ -1135,9 +1297,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1704,23 +1866,176 @@
       </c>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" ht="49" x14ac:dyDescent="0.35">
+      <c r="B30" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" ht="98" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2015</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" ht="118" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1999</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" ht="67.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2012</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1997</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="K34" s="1"/>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B40" s="7"/>
+    <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="90" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="D36" s="1">
+        <v>2023</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>154</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B38" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D38" s="1">
+        <v>2010</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="67.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B39" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="D39" s="1">
+        <v>2021</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="67.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B40" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2018</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>162</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
@@ -1812,11 +2127,12 @@
     <hyperlink ref="J21" r:id="rId4" xr:uid="{CDC23153-E9B4-4648-B970-3EF7B21294EE}"/>
     <hyperlink ref="J2" r:id="rId5" xr:uid="{23FBF90A-2CF3-4F48-B0AB-B8009FFB5CBA}"/>
     <hyperlink ref="J10" r:id="rId6" xr:uid="{614A66CE-0829-481F-AFAF-A492F6B5D9FE}"/>
+    <hyperlink ref="B31" r:id="rId7" display="https://www.sciencedirect.com/science/article/pii/S1574119214001564" xr:uid="{EE8E0444-AE6C-4B46-A451-0B8E5DA6849B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
diary update, did some overleaf writin
</commit_message>
<xml_diff>
--- a/ResearchDiary/RelatedWorkTabelle.xlsx
+++ b/ResearchDiary/RelatedWorkTabelle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmaer\Documents\FH\Projects\MasterArbeit\mmt-masterarbeit-david-maerzendorfer\ResearchDiary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127D1751-6D4A-4295-80BA-D61D97391E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD8260A-C4B0-4391-B020-89AF4064C7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,9 +215,6 @@
     <t>zaman, anslow, rhee</t>
   </si>
   <si>
-    <t>Transitional Augmented Reality Navigation for Live Captured Scenes</t>
-  </si>
-  <si>
     <t>Tatzgern, et al.</t>
   </si>
   <si>
@@ -525,6 +522,9 @@
   </si>
   <si>
     <t>method for manipulating distant things in VR</t>
+  </si>
+  <si>
+    <t>Transitional Augmented Reality Navigation for Live Captured Scenes+[@Paper]</t>
   </si>
 </sst>
 </file>
@@ -1297,9 +1297,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1567,474 +1567,474 @@
     </row>
     <row r="13" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>163</v>
       </c>
       <c r="D13" s="1">
         <v>2014</v>
       </c>
       <c r="I13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D14" s="1">
         <v>2018</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J14" s="1" t="s">
         <v>64</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15" s="1">
         <v>2024</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
         <v>73</v>
-      </c>
-      <c r="B16" t="s">
-        <v>74</v>
       </c>
       <c r="D16" s="1">
         <v>2023</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D17" s="1">
         <v>2021</v>
       </c>
       <c r="I17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D18" s="1">
         <v>2022</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D19" s="1">
         <v>2015</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K19" s="1"/>
     </row>
     <row r="20" spans="1:11" ht="40" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D20" s="1">
         <v>2018</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K20" s="1"/>
     </row>
     <row r="21" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="1">
         <v>2017</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="20" t="s">
         <v>97</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>98</v>
       </c>
       <c r="D22" s="1">
         <v>2017</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:11" ht="40" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D23" s="1">
         <v>2018</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D24" s="1">
         <v>2002</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D25" s="1">
         <v>2022</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D26" s="1">
         <v>2016</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:11" ht="52.5" x14ac:dyDescent="0.35">
       <c r="B27" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D27" s="1">
         <v>2017</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K27" s="1"/>
     </row>
     <row r="28" spans="1:11" ht="52.5" x14ac:dyDescent="0.35">
       <c r="B28" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D28" s="1">
         <v>2018</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K28" s="1"/>
     </row>
     <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.35">
       <c r="A29" s="22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D29" s="1">
         <v>2018</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K29" s="1"/>
     </row>
     <row r="30" spans="1:11" ht="49" x14ac:dyDescent="0.35">
       <c r="B30" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K30" s="1"/>
     </row>
     <row r="31" spans="1:11" ht="98" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="24" t="s">
         <v>130</v>
-      </c>
-      <c r="B31" s="24" t="s">
-        <v>131</v>
       </c>
       <c r="D31" s="1">
         <v>2015</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" ht="118" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" ht="88.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D32" s="1">
         <v>1999</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="K32" s="1"/>
     </row>
     <row r="33" spans="1:11" ht="67.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D33" s="1">
         <v>2012</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K33" s="1"/>
     </row>
     <row r="34" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D34" s="1">
         <v>1997</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K34" s="1"/>
     </row>
     <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D35" s="1">
         <v>2021</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="90" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D36" s="1">
         <v>2023</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D38" s="1">
         <v>2010</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="67.5" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D39" s="1">
         <v>2021</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="67.5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D40" s="1">
         <v>2018</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="J40" s="1" t="s">
         <v>162</v>
+      </c>
+      <c r="J40" s="7" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2128,11 +2128,14 @@
     <hyperlink ref="J2" r:id="rId5" xr:uid="{23FBF90A-2CF3-4F48-B0AB-B8009FFB5CBA}"/>
     <hyperlink ref="J10" r:id="rId6" xr:uid="{614A66CE-0829-481F-AFAF-A492F6B5D9FE}"/>
     <hyperlink ref="B31" r:id="rId7" display="https://www.sciencedirect.com/science/article/pii/S1574119214001564" xr:uid="{EE8E0444-AE6C-4B46-A451-0B8E5DA6849B}"/>
+    <hyperlink ref="J40" r:id="rId8" xr:uid="{82B84AAE-296E-45F5-88A1-86E77CE11849}"/>
+    <hyperlink ref="J32" r:id="rId9" xr:uid="{6CB365ED-AE11-4489-AB4A-1A28C0AA5012}"/>
+    <hyperlink ref="J14" r:id="rId10" xr:uid="{D5B8BD31-5A71-42BB-99CA-842BAACDA67E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
   <tableParts count="1">
-    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId12"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
some tinkering on orbit cameras and diary update
</commit_message>
<xml_diff>
--- a/ResearchDiary/RelatedWorkTabelle.xlsx
+++ b/ResearchDiary/RelatedWorkTabelle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmaer\Documents\FH\Projects\MasterArbeit\mmt-masterarbeit-david-maerzendorfer\ResearchDiary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD8260A-C4B0-4391-B020-89AF4064C7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB415B60-F70F-4A00-8A6B-560E709F6F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="172">
   <si>
     <t>Paper</t>
   </si>
@@ -525,13 +525,37 @@
   </si>
   <si>
     <t>Transitional Augmented Reality Navigation for Live Captured Scenes+[@Paper]</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/3611023</t>
+  </si>
+  <si>
+    <t>A Matter of Perspective: Designing Immersive Character Transitions for Virtual Reality Games</t>
+  </si>
+  <si>
+    <t>viewpoint transitions in narrative games -&gt; also nice references to embodiment, body ownership, race/age/gender of avatars etc. :)</t>
+  </si>
+  <si>
+    <t>Sebastian Cmentowski et al.</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/3411764.3445685</t>
+  </si>
+  <si>
+    <t>Henning phol et al.</t>
+  </si>
+  <si>
+    <t>cool as method for distant object interaction and more like viewpoints etc :)</t>
+  </si>
+  <si>
+    <t>Poros: Configurable Proxies for Distant Interactions in VR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -692,6 +716,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -744,7 +774,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -826,6 +856,9 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -976,8 +1009,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F5384B4F-E58A-4FDF-9026-5EF3EE172CA3}" name="Tabelle2" displayName="Tabelle2" ref="A1:J41" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
-  <autoFilter ref="A1:J41" xr:uid="{622A20CF-99C6-4D06-B80E-EDF4CD2ACC21}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F5384B4F-E58A-4FDF-9026-5EF3EE172CA3}" name="Tabelle2" displayName="Tabelle2" ref="A1:J42" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+  <autoFilter ref="A1:J42" xr:uid="{622A20CF-99C6-4D06-B80E-EDF4CD2ACC21}"/>
   <tableColumns count="10">
     <tableColumn id="10" xr3:uid="{3982B8B8-D4C3-477E-982F-5AF76F683E58}" name="Authors" dataDxfId="33"/>
     <tableColumn id="1" xr3:uid="{EA04F39E-73D9-490A-863B-16A3A0920927}" name="Paper" dataDxfId="32"/>
@@ -1295,11 +1328,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J38" sqref="J38"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1482,7 +1515,7 @@
       <c r="I8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="7" t="s">
         <v>40</v>
       </c>
       <c r="K8" s="1"/>
@@ -1500,7 +1533,7 @@
       <c r="I9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="7" t="s">
         <v>44</v>
       </c>
       <c r="K9" s="1"/>
@@ -1539,7 +1572,7 @@
       <c r="I11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="7" t="s">
         <v>54</v>
       </c>
       <c r="K11" s="1"/>
@@ -1560,7 +1593,7 @@
       <c r="I12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="7" t="s">
         <v>58</v>
       </c>
       <c r="K12" s="1"/>
@@ -1614,7 +1647,7 @@
       <c r="I15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="J15" s="7" t="s">
         <v>67</v>
       </c>
       <c r="K15" s="1"/>
@@ -1813,7 +1846,7 @@
       <c r="I26" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="J26" s="7" t="s">
         <v>111</v>
       </c>
       <c r="K26" s="1"/>
@@ -1980,7 +2013,7 @@
       <c r="I36" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="J36" s="7" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2035,6 +2068,40 @@
       </c>
       <c r="J40" s="7" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="118" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B41" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="D41" s="1">
+        <v>2023</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="88.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B42" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="D42" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2131,11 +2198,18 @@
     <hyperlink ref="J40" r:id="rId8" xr:uid="{82B84AAE-296E-45F5-88A1-86E77CE11849}"/>
     <hyperlink ref="J32" r:id="rId9" xr:uid="{6CB365ED-AE11-4489-AB4A-1A28C0AA5012}"/>
     <hyperlink ref="J14" r:id="rId10" xr:uid="{D5B8BD31-5A71-42BB-99CA-842BAACDA67E}"/>
+    <hyperlink ref="J8" r:id="rId11" xr:uid="{E3DD1CBF-4264-420C-AC0B-4322FAB20314}"/>
+    <hyperlink ref="J9" r:id="rId12" xr:uid="{9CCCF8F8-5CFC-44A9-98C6-3F34ED15EAAB}"/>
+    <hyperlink ref="J11" r:id="rId13" xr:uid="{CD210EBB-6965-453D-9FBB-D7C8B65A1DA7}"/>
+    <hyperlink ref="J12" r:id="rId14" xr:uid="{17D3CAD1-620D-4FEF-B988-6AF8826FE6E5}"/>
+    <hyperlink ref="J15" r:id="rId15" xr:uid="{E5A11ADD-9034-4FF5-9A06-29DCD7659C0E}"/>
+    <hyperlink ref="J26" r:id="rId16" xr:uid="{F369DC0D-6AC8-4A70-A14D-957206F04172}"/>
+    <hyperlink ref="J36" r:id="rId17" xr:uid="{05B028EC-0D3A-4234-A9F9-56BBE47387F9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
   <tableParts count="1">
-    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId19"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
did some study/task planning, made point of interest script, fixed control table bugs
</commit_message>
<xml_diff>
--- a/ResearchDiary/RelatedWorkTabelle.xlsx
+++ b/ResearchDiary/RelatedWorkTabelle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmaer\Documents\FH\Projects\MasterArbeit\mmt-masterarbeit-david-maerzendorfer\ResearchDiary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB415B60-F70F-4A00-8A6B-560E709F6F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C2CFF1-CE32-4DD7-BAEA-2058D335BAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="180">
   <si>
     <t>Paper</t>
   </si>
@@ -549,13 +549,37 @@
   </si>
   <si>
     <t>Poros: Configurable Proxies for Distant Interactions in VR</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/abs/10.1145/3379350.3416188</t>
+  </si>
+  <si>
+    <t>paper on build in questionnare toolkit in VR</t>
+  </si>
+  <si>
+    <t>The Virtual Reality Questionnaire Toolkit</t>
+  </si>
+  <si>
+    <t>Martin Feick et al.</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/301558848_A_Questionnaire_to_Measure_the_User_Experience_in_Immersive_Virtual_Environments</t>
+  </si>
+  <si>
+    <t>questionnaire stuff to measure user experience</t>
+  </si>
+  <si>
+    <t>A Questionnaire to Measure the User Experience in Immersive Virtual Environments</t>
+  </si>
+  <si>
+    <t>katy tcha-tokey et al.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -722,6 +746,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF111111"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -774,7 +811,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -858,6 +895,12 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1009,8 +1052,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F5384B4F-E58A-4FDF-9026-5EF3EE172CA3}" name="Tabelle2" displayName="Tabelle2" ref="A1:J42" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
-  <autoFilter ref="A1:J42" xr:uid="{622A20CF-99C6-4D06-B80E-EDF4CD2ACC21}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F5384B4F-E58A-4FDF-9026-5EF3EE172CA3}" name="Tabelle2" displayName="Tabelle2" ref="A1:J44" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+  <autoFilter ref="A1:J44" xr:uid="{622A20CF-99C6-4D06-B80E-EDF4CD2ACC21}"/>
   <tableColumns count="10">
     <tableColumn id="10" xr3:uid="{3982B8B8-D4C3-477E-982F-5AF76F683E58}" name="Authors" dataDxfId="33"/>
     <tableColumn id="1" xr3:uid="{EA04F39E-73D9-490A-863B-16A3A0920927}" name="Paper" dataDxfId="32"/>
@@ -1328,11 +1371,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1452,7 +1495,7 @@
       <c r="I5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="7" t="s">
         <v>23</v>
       </c>
       <c r="K5" s="1"/>
@@ -1894,7 +1937,7 @@
       <c r="I29" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="J29" s="7" t="s">
         <v>120</v>
       </c>
       <c r="K29" s="1"/>
@@ -1960,7 +2003,7 @@
       <c r="I33" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="J33" s="7" t="s">
         <v>135</v>
       </c>
       <c r="K33" s="1"/>
@@ -2087,7 +2130,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" ht="59" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>169</v>
       </c>
@@ -2102,6 +2145,40 @@
       </c>
       <c r="J42" s="1" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="60" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B43" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="D43" s="1">
+        <v>2020</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="67.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B44" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="D44" s="1">
+        <v>2016</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2205,11 +2282,14 @@
     <hyperlink ref="J15" r:id="rId15" xr:uid="{E5A11ADD-9034-4FF5-9A06-29DCD7659C0E}"/>
     <hyperlink ref="J26" r:id="rId16" xr:uid="{F369DC0D-6AC8-4A70-A14D-957206F04172}"/>
     <hyperlink ref="J36" r:id="rId17" xr:uid="{05B028EC-0D3A-4234-A9F9-56BBE47387F9}"/>
+    <hyperlink ref="J5" r:id="rId18" xr:uid="{B59C9DB2-D175-4C02-9665-B463AFFCBCF0}"/>
+    <hyperlink ref="J29" r:id="rId19" xr:uid="{55D1C017-F8C0-47AE-A2E0-6001D5A1CE9B}"/>
+    <hyperlink ref="J33" r:id="rId20" xr:uid="{2742FD66-0FFB-453A-97B4-C9BCD1A11C48}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
   <tableParts count="1">
-    <tablePart r:id="rId19"/>
+    <tablePart r:id="rId22"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
first version of hover cam
</commit_message>
<xml_diff>
--- a/ResearchDiary/RelatedWorkTabelle.xlsx
+++ b/ResearchDiary/RelatedWorkTabelle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmaer\Documents\FH\Projects\MasterArbeit\mmt-masterarbeit-david-maerzendorfer\ResearchDiary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C2CFF1-CE32-4DD7-BAEA-2058D335BAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5BE850-BA68-4670-8892-15B3566938DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1020" yWindow="1010" windowWidth="21640" windowHeight="11200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="239">
   <si>
     <t>Paper</t>
   </si>
@@ -573,13 +573,272 @@
   </si>
   <si>
     <t>katy tcha-tokey et al.</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/571985.572000</t>
+  </si>
+  <si>
+    <r>
+      <t>StyleCam: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="24"/>
+        <color rgb="FF000000"/>
+        <rFont val="Unset"/>
+      </rPr>
+      <t>interactive stylized 3D navigation using integrated spatial &amp; temporal controls</t>
+    </r>
+  </si>
+  <si>
+    <t>Nicholas Burtnyk et al.</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/1665817.1665820</t>
+  </si>
+  <si>
+    <r>
+      <t>Camera control in computer graphics: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="24"/>
+        <color rgb="FF000000"/>
+        <rFont val="Unset"/>
+      </rPr>
+      <t>models, techniques and applications</t>
+    </r>
+  </si>
+  <si>
+    <t>Marc Christie et al.</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/1613858.1613899</t>
+  </si>
+  <si>
+    <t>A study of direct versus planned 3D camera manipulation on touch-based mobile phones</t>
+  </si>
+  <si>
+    <t>Fabrice Decle et al.</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/1053427.1053439</t>
+  </si>
+  <si>
+    <r>
+      <t>HoverCam: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="24"/>
+        <color rgb="FF000000"/>
+        <rFont val="Unset"/>
+      </rPr>
+      <t>interactive 3D navigation for proximal object inspection</t>
+    </r>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/1342250.1342253</t>
+  </si>
+  <si>
+    <r>
+      <t>ViewCube: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="24"/>
+        <color rgb="FF000000"/>
+        <rFont val="Unset"/>
+      </rPr>
+      <t>a 3D orientation indicator and controller</t>
+    </r>
+  </si>
+  <si>
+    <t>Azam Khan et al.</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/1507149.1507151</t>
+  </si>
+  <si>
+    <t>Multiscale 3D navigation</t>
+  </si>
+  <si>
+    <t>James McCrae et al.</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/1622176.1622190</t>
+  </si>
+  <si>
+    <t>A screen-space formulation for 2D and 3D direct manipulation</t>
+  </si>
+  <si>
+    <t>Jason L. Reisman et al.</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/365024.365307</t>
+  </si>
+  <si>
+    <r>
+      <t>Exploring 3D navigation: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="24"/>
+        <color rgb="FF000000"/>
+        <rFont val="Unset"/>
+      </rPr>
+      <t>combining speed-coupled flying with orbiting</t>
+    </r>
+  </si>
+  <si>
+    <t>Desney S. Tan et al.</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.5555/601671.601708</t>
+  </si>
+  <si>
+    <t>Distance-field based skeletons for virtual navigation</t>
+  </si>
+  <si>
+    <t>Ming Wan et al.</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/300523.300546</t>
+  </si>
+  <si>
+    <t>UniCam—2D gestural camera controls for 3D environments</t>
+  </si>
+  <si>
+    <t>Robert Zeleznik et al.</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/4483791</t>
+  </si>
+  <si>
+    <t>A Taxonomy of 3D Occlusion Management for Visualization</t>
+  </si>
+  <si>
+    <t>Niklas Elmqvist et al.</t>
+  </si>
+  <si>
+    <t>https://inria.hal.science/hal-00789413/file/EG2013-STAR.pdf</t>
+  </si>
+  <si>
+    <t>A Survey of Interaction Techniques for Interactive 3D Environments</t>
+  </si>
+  <si>
+    <t>Jacek Jankowski et al.</t>
+  </si>
+  <si>
+    <t>object centered approach with certain view areas where user can control in more detail. An animated camera tracking transition is used to change to another of such free cam areas. The transition can be stopped and scrubbed via a button press.</t>
+  </si>
+  <si>
+    <t>different approaches for camera control -&gt; seems to go in the broader basics on the topic. Maybe worth a rough read</t>
+  </si>
+  <si>
+    <t>rotating viewpoints/orbit cams? With a touch based input interface. Also got a user study -&gt; even though short check out how they structured it (missing hypothesis tho I think)</t>
+  </si>
+  <si>
+    <t>hover-cam, a system that keeps a cam always a certain distance from an object with smooth moving on it</t>
+  </si>
+  <si>
+    <t>a widget to make orientation in 3d space easier when viewing an object. The view-cube allows to jump to top down, front, side, etc. views.</t>
+  </si>
+  <si>
+    <t>navigation of 3d scenes with different scales, usage of a 'cube map' which is an improvement of the hoverCam. This allows for just selecting a point on the cube map and the cam flies there; vergleich google maps; interesting: "Another school of thought proceeds that the authors of a virtual
+environment know best what the points of interest are, and should
+therefore assist users in reaching them. [Haik et al. 2002] showed
+that by sacrificing freedom of navigation, users completed navigation tasks more quickly and were able to locate and view selected
+features of a scene without getting lost or disoriented. "</t>
+  </si>
+  <si>
+    <t>rotate scale translate (rst) interactions in 3d, touch/finger gestures</t>
+  </si>
+  <si>
+    <t>view navigation kind of like flying a plane. If fast enough an pulling up camera rises etc. with added orbit cam features</t>
+  </si>
+  <si>
+    <t>for automatic planning a flight path in virtual environment</t>
+  </si>
+  <si>
+    <t>controlling a 3d cam with just a 2d mouse input</t>
+  </si>
+  <si>
+    <t>human perception in regard to occlusion. Looks into five design patterns, one of which is multiple viewpoints -&gt; says its sometimes powerfull but has drawback of tacking screenspace away from main view. Often used in construction etc or eG in blender 3d. often predefined views? user cannot change. but he can with my approach :P user can also decide how many views he/she needs.</t>
+  </si>
+  <si>
+    <t>alround good paper with nice references on interaction techniques for interactive 3d environments. Pretty much references everything above -&gt; briefly look over listed stuff and check if there is something semi automatic (other than hover cam) that I could use for my orbit cam
+also goes into detail on object selection via raycast</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/3204493.3204555</t>
+  </si>
+  <si>
+    <r>
+      <t>Anyorbit: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="24"/>
+        <color rgb="FF000000"/>
+        <rFont val="Unset"/>
+      </rPr>
+      <t>orbital navigation in virtual environments with eye-tracking</t>
+    </r>
+  </si>
+  <si>
+    <t>an orbit camera but the center is determined via eye tracking</t>
+  </si>
+  <si>
+    <t>benjamin I. Outram et al.</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/7025813</t>
+  </si>
+  <si>
+    <t>similar to hoverCam but on gpu</t>
+  </si>
+  <si>
+    <t>ShellCam: Interactive geometry-aware virtual camera control</t>
+  </si>
+  <si>
+    <t>Tamy Boubekeur</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/abs/10.1145/2807442.2807496</t>
+  </si>
+  <si>
+    <r>
+      <t>SHOCam: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="24"/>
+        <color rgb="FF000000"/>
+        <rFont val="Unset"/>
+      </rPr>
+      <t>A 3D Orbiting Algorithm</t>
+    </r>
+  </si>
+  <si>
+    <t>yet another improved hover cam</t>
+  </si>
+  <si>
+    <t>michael ortega et al.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -759,6 +1018,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Unset"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1052,8 +1317,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F5384B4F-E58A-4FDF-9026-5EF3EE172CA3}" name="Tabelle2" displayName="Tabelle2" ref="A1:J44" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
-  <autoFilter ref="A1:J44" xr:uid="{622A20CF-99C6-4D06-B80E-EDF4CD2ACC21}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F5384B4F-E58A-4FDF-9026-5EF3EE172CA3}" name="Tabelle2" displayName="Tabelle2" ref="A1:J59" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+  <autoFilter ref="A1:J59" xr:uid="{622A20CF-99C6-4D06-B80E-EDF4CD2ACC21}"/>
   <tableColumns count="10">
     <tableColumn id="10" xr3:uid="{3982B8B8-D4C3-477E-982F-5AF76F683E58}" name="Authors" dataDxfId="33"/>
     <tableColumn id="1" xr3:uid="{EA04F39E-73D9-490A-863B-16A3A0920927}" name="Paper" dataDxfId="32"/>
@@ -1371,14 +1636,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="17.90625" style="1" customWidth="1"/>
     <col min="2" max="2" width="59.26953125" style="1" customWidth="1"/>
@@ -1392,7 +1657,7 @@
     <col min="12" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1425,7 +1690,7 @@
       </c>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="29">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1446,7 +1711,7 @@
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1458,7 +1723,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1479,7 +1744,7 @@
       </c>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="29">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -1500,7 +1765,7 @@
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="29">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -1521,7 +1786,7 @@
       </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="35">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -1542,7 +1807,7 @@
       </c>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="40" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="40">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -1563,7 +1828,7 @@
       </c>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="40" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="40">
       <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
@@ -1581,7 +1846,7 @@
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="45">
       <c r="A10" s="1" t="s">
         <v>49</v>
       </c>
@@ -1599,7 +1864,7 @@
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="45">
       <c r="A11" s="1" t="s">
         <v>53</v>
       </c>
@@ -1620,7 +1885,7 @@
       </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="40" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="40">
       <c r="A12" s="1" t="s">
         <v>59</v>
       </c>
@@ -1641,7 +1906,7 @@
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="58">
       <c r="A13" s="1" t="s">
         <v>60</v>
       </c>
@@ -1659,7 +1924,7 @@
       </c>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="29">
       <c r="A14" s="1" t="s">
         <v>66</v>
       </c>
@@ -1677,7 +1942,7 @@
       </c>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="43.5">
       <c r="A15" s="1" t="s">
         <v>69</v>
       </c>
@@ -1695,7 +1960,7 @@
       </c>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="43.5">
       <c r="A16" s="1" t="s">
         <v>72</v>
       </c>
@@ -1713,7 +1978,7 @@
       </c>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="45">
       <c r="A17" s="1" t="s">
         <v>76</v>
       </c>
@@ -1731,7 +1996,7 @@
       </c>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="43.5">
       <c r="A18" s="1" t="s">
         <v>82</v>
       </c>
@@ -1749,7 +2014,7 @@
       </c>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="58">
       <c r="A19" s="1" t="s">
         <v>84</v>
       </c>
@@ -1767,7 +2032,7 @@
       </c>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" ht="40" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="40">
       <c r="A20" s="1" t="s">
         <v>89</v>
       </c>
@@ -1785,7 +2050,7 @@
       </c>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="58">
       <c r="A21" s="1" t="s">
         <v>94</v>
       </c>
@@ -1804,7 +2069,7 @@
       </c>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11">
       <c r="A22" s="1" t="s">
         <v>96</v>
       </c>
@@ -1822,7 +2087,7 @@
       </c>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" ht="40" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="40">
       <c r="A23" s="1" t="s">
         <v>84</v>
       </c>
@@ -1840,7 +2105,7 @@
       </c>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="29">
       <c r="A24" s="1" t="s">
         <v>105</v>
       </c>
@@ -1861,7 +2126,7 @@
       </c>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" ht="60">
       <c r="A25" s="1" t="s">
         <v>108</v>
       </c>
@@ -1879,7 +2144,7 @@
       </c>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="43.5">
       <c r="B26" t="s">
         <v>112</v>
       </c>
@@ -1894,7 +2159,7 @@
       </c>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="52.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" ht="52.5">
       <c r="B27" s="21" t="s">
         <v>116</v>
       </c>
@@ -1909,7 +2174,7 @@
       </c>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" ht="52.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" ht="52.5">
       <c r="B28" s="21" t="s">
         <v>118</v>
       </c>
@@ -1924,7 +2189,7 @@
       </c>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" ht="45">
       <c r="A29" s="22" t="s">
         <v>121</v>
       </c>
@@ -1942,7 +2207,7 @@
       </c>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" ht="49" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" ht="49">
       <c r="B30" s="24" t="s">
         <v>126</v>
       </c>
@@ -1954,7 +2219,7 @@
       </c>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" ht="98" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" ht="98">
       <c r="A31" s="1" t="s">
         <v>129</v>
       </c>
@@ -1972,7 +2237,7 @@
       </c>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" ht="88.5">
       <c r="A32" s="1" t="s">
         <v>133</v>
       </c>
@@ -1990,7 +2255,7 @@
       </c>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" ht="67.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" ht="67.5">
       <c r="A33" s="1" t="s">
         <v>138</v>
       </c>
@@ -2008,7 +2273,7 @@
       </c>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" ht="43.5">
       <c r="A34" s="1" t="s">
         <v>142</v>
       </c>
@@ -2026,7 +2291,7 @@
       </c>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" ht="60">
       <c r="A35" s="1" t="s">
         <v>146</v>
       </c>
@@ -2043,7 +2308,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="90" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" ht="90">
       <c r="A36" s="1" t="s">
         <v>150</v>
       </c>
@@ -2060,7 +2325,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" ht="43.5">
       <c r="B37" t="s">
         <v>153</v>
       </c>
@@ -2071,7 +2336,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" ht="43.5">
       <c r="B38" s="1" t="s">
         <v>155</v>
       </c>
@@ -2082,7 +2347,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="67.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" ht="67.5">
       <c r="A39" s="1" t="s">
         <v>158</v>
       </c>
@@ -2096,7 +2361,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="67.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" ht="67.5">
       <c r="A40" s="1" t="s">
         <v>160</v>
       </c>
@@ -2113,7 +2378,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="118" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" ht="118">
       <c r="A41" s="1" t="s">
         <v>167</v>
       </c>
@@ -2130,7 +2395,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="59" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" ht="59">
       <c r="A42" s="1" t="s">
         <v>169</v>
       </c>
@@ -2147,7 +2412,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="60" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" ht="60">
       <c r="A43" s="1" t="s">
         <v>175</v>
       </c>
@@ -2164,7 +2429,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="67.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" ht="67.5">
       <c r="A44" s="1" t="s">
         <v>179</v>
       </c>
@@ -2179,6 +2444,261 @@
       </c>
       <c r="J44" s="1" t="s">
         <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="120">
+      <c r="A45" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B45" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="D45" s="1">
+        <v>2002</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="150">
+      <c r="A46" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B46" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="D46" s="1">
+        <v>2009</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="J46" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="120">
+      <c r="A47" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B47" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="D47" s="1">
+        <v>2009</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J47" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="90">
+      <c r="A48" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B48" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="D48" s="1">
+        <v>2005</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="J48" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="60">
+      <c r="A49" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B49" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="D49" s="1">
+        <v>2008</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J49" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="145">
+      <c r="A50" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B50" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="D50" s="1">
+        <v>2009</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="J50" s="7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="90">
+      <c r="A51" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B51" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="D51" s="1">
+        <v>2009</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="120">
+      <c r="A52" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B52" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="D52" s="1">
+        <v>2001</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="J52" s="7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="90">
+      <c r="A53" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B53" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="D53" s="1">
+        <v>2001</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J53" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="90">
+      <c r="A54" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B54" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="D54" s="1">
+        <v>1999</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J54" s="7" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="87">
+      <c r="A55" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="D55" s="1">
+        <v>2023</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="J55" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="72.5">
+      <c r="A56" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B56" t="s">
+        <v>213</v>
+      </c>
+      <c r="D56" s="1">
+        <v>2013</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J56" s="7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="90">
+      <c r="A57" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B57" s="30" t="s">
+        <v>228</v>
+      </c>
+      <c r="D57" s="1">
+        <v>2018</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="40">
+      <c r="A58" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="D58" s="1">
+        <v>2014</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="60">
+      <c r="A59" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B59" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="D59" s="1">
+        <v>2015</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -2285,11 +2805,23 @@
     <hyperlink ref="J5" r:id="rId18" xr:uid="{B59C9DB2-D175-4C02-9665-B463AFFCBCF0}"/>
     <hyperlink ref="J29" r:id="rId19" xr:uid="{55D1C017-F8C0-47AE-A2E0-6001D5A1CE9B}"/>
     <hyperlink ref="J33" r:id="rId20" xr:uid="{2742FD66-0FFB-453A-97B4-C9BCD1A11C48}"/>
+    <hyperlink ref="J45" r:id="rId21" xr:uid="{5E3E0467-6A02-43DA-A731-EC4BBD855118}"/>
+    <hyperlink ref="J47" r:id="rId22" xr:uid="{3D5DCB8D-835C-4233-A0CC-788CF5B2ADA3}"/>
+    <hyperlink ref="J48" r:id="rId23" xr:uid="{846BB1C8-309F-4347-91EC-BBC56C203244}"/>
+    <hyperlink ref="J49" r:id="rId24" xr:uid="{DF9166E9-0BE9-4B8A-8E23-3ED030E31391}"/>
+    <hyperlink ref="J46" r:id="rId25" xr:uid="{5BCF611B-F09F-4779-B857-71B7A16561E0}"/>
+    <hyperlink ref="J50" r:id="rId26" xr:uid="{F66EFC32-1857-4F36-ADD9-8CE6A3C40BC9}"/>
+    <hyperlink ref="J51" r:id="rId27" xr:uid="{DA73176B-1168-4BDD-BEFD-EF6B4616C242}"/>
+    <hyperlink ref="J52" r:id="rId28" xr:uid="{DD278C41-3085-4B6B-9BC6-EB0927CF7036}"/>
+    <hyperlink ref="J53" r:id="rId29" xr:uid="{14C04C01-A768-423E-8E3A-614977A0F0BA}"/>
+    <hyperlink ref="J54" r:id="rId30" xr:uid="{13529C30-E1D0-4852-B670-855209850AC8}"/>
+    <hyperlink ref="J55" r:id="rId31" xr:uid="{84112BF8-FAB9-4F73-A8E6-63A812A59F32}"/>
+    <hyperlink ref="J56" r:id="rId32" xr:uid="{FAB1351F-74E8-44A0-ADEF-6B18DD0E863F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>
   <tableParts count="1">
-    <tablePart r:id="rId22"/>
+    <tablePart r:id="rId34"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2302,7 +2834,7 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="45.26953125" style="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" customWidth="1"/>
@@ -2314,7 +2846,7 @@
     <col min="10" max="10" width="64.1796875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="29">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2346,146 +2878,146 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="A11" s="1"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1">
       <c r="A33" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1">
       <c r="A49" s="1"/>
     </row>
   </sheetData>
@@ -2555,7 +3087,7 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="55" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.26953125" style="1" customWidth="1"/>
@@ -2566,7 +3098,7 @@
     <col min="10" max="10" width="48" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2598,92 +3130,92 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10">
       <c r="A12" s="1"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10">
       <c r="A14" s="1"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10">
       <c r="A16" s="1"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2">
       <c r="A25" s="1"/>
       <c r="B25" s="8"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2">
       <c r="A28" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated study manager to use new task setup, needs testing however
</commit_message>
<xml_diff>
--- a/ResearchDiary/RelatedWorkTabelle.xlsx
+++ b/ResearchDiary/RelatedWorkTabelle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmaer\Documents\FH\Projects\MasterArbeit\mmt-masterarbeit-david-maerzendorfer\ResearchDiary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5BE850-BA68-4670-8892-15B3566938DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8FBC23-4CC2-44DF-B6E7-68AA12692B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1020" yWindow="1010" windowWidth="21640" windowHeight="11200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="254">
   <si>
     <t>Paper</t>
   </si>
@@ -833,12 +833,57 @@
   <si>
     <t>michael ortega et al.</t>
   </si>
+  <si>
+    <t>https://www.igroup.org/pq/ipq/download.php</t>
+  </si>
+  <si>
+    <t>presence questionnaire used by hoppe for perspective continuum</t>
+  </si>
+  <si>
+    <t>ipq</t>
+  </si>
+  <si>
+    <t>https://www.frontiersin.org/journals/robotics-and-ai/articles/10.3389/frobt.2017.00033/full</t>
+  </si>
+  <si>
+    <t>First- and Third-Person Perspectives in Immersive Virtual Environments: Presence and Performance Analysis of Embodied Users</t>
+  </si>
+  <si>
+    <t>Geoffrey gorisse et al.</t>
+  </si>
+  <si>
+    <t>embodiment questionnaire used by hoppe for perspective continuum</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/3582700.3582706</t>
+  </si>
+  <si>
+    <t>shadow clones, user controls multiple things at the same time</t>
+  </si>
+  <si>
+    <t>ShadowClones: an Interface to Maintain a Multiple Sense of Body-space Coordination in Multiple Visual Perspectives</t>
+  </si>
+  <si>
+    <t>kazuma takada et al.</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/10108469</t>
+  </si>
+  <si>
+    <t>paper on switching embodiment and how to do it smoothly, they link it to physical action</t>
+  </si>
+  <si>
+    <t>I'm Transforming! Effects of Visual Transitions to Change of Avatar on the Sense of Embodiment in AR</t>
+  </si>
+  <si>
+    <t>riku otono et al.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1024,6 +1069,13 @@
       <color rgb="FF000000"/>
       <name val="Unset"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1076,7 +1128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1167,6 +1219,9 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1317,8 +1372,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F5384B4F-E58A-4FDF-9026-5EF3EE172CA3}" name="Tabelle2" displayName="Tabelle2" ref="A1:J59" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
-  <autoFilter ref="A1:J59" xr:uid="{622A20CF-99C6-4D06-B80E-EDF4CD2ACC21}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F5384B4F-E58A-4FDF-9026-5EF3EE172CA3}" name="Tabelle2" displayName="Tabelle2" ref="A1:J63" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+  <autoFilter ref="A1:J63" xr:uid="{622A20CF-99C6-4D06-B80E-EDF4CD2ACC21}"/>
   <tableColumns count="10">
     <tableColumn id="10" xr3:uid="{3982B8B8-D4C3-477E-982F-5AF76F683E58}" name="Authors" dataDxfId="33"/>
     <tableColumn id="1" xr3:uid="{EA04F39E-73D9-490A-863B-16A3A0920927}" name="Paper" dataDxfId="32"/>
@@ -1636,11 +1691,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L62" sqref="L62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -1739,7 +1794,7 @@
       <c r="I4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="7" t="s">
         <v>17</v>
       </c>
       <c r="K4" s="1"/>
@@ -2232,7 +2287,7 @@
       <c r="I31" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="J31" s="7" t="s">
         <v>127</v>
       </c>
       <c r="K31" s="1"/>
@@ -2408,7 +2463,7 @@
       <c r="I42" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="J42" s="7" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2663,7 +2718,7 @@
       <c r="I57" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="J57" s="1" t="s">
+      <c r="J57" s="7" t="s">
         <v>227</v>
       </c>
     </row>
@@ -2680,7 +2735,7 @@
       <c r="I58" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="J58" s="1" t="s">
+      <c r="J58" s="7" t="s">
         <v>231</v>
       </c>
     </row>
@@ -2697,8 +2752,70 @@
       <c r="I59" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="J59" s="1" t="s">
+      <c r="J59" s="7" t="s">
         <v>235</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="B60" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="J60" s="7" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="31">
+      <c r="A61" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B61" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="D61" s="1">
+        <v>2017</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="J61" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="180">
+      <c r="A62" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B62" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="D62" s="1">
+        <v>2023</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="60">
+      <c r="A63" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="D63" s="1">
+        <v>2023</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -2817,11 +2934,19 @@
     <hyperlink ref="J54" r:id="rId30" xr:uid="{13529C30-E1D0-4852-B670-855209850AC8}"/>
     <hyperlink ref="J55" r:id="rId31" xr:uid="{84112BF8-FAB9-4F73-A8E6-63A812A59F32}"/>
     <hyperlink ref="J56" r:id="rId32" xr:uid="{FAB1351F-74E8-44A0-ADEF-6B18DD0E863F}"/>
+    <hyperlink ref="J42" r:id="rId33" xr:uid="{B013429A-9046-47E2-A8FC-A845E2F96690}"/>
+    <hyperlink ref="J58" r:id="rId34" xr:uid="{520F7075-0615-49C0-B7B5-52010D20517D}"/>
+    <hyperlink ref="J59" r:id="rId35" xr:uid="{84AA1D8E-9528-4B8F-A2AF-ED507037375B}"/>
+    <hyperlink ref="J57" r:id="rId36" xr:uid="{3252D64B-DBE4-41AF-85A3-D8070393E161}"/>
+    <hyperlink ref="J31" r:id="rId37" xr:uid="{26827437-0288-4511-9B57-20CECC079807}"/>
+    <hyperlink ref="J4" r:id="rId38" xr:uid="{1F3018DF-9A45-4184-8FF7-66A67C65CF9B}"/>
+    <hyperlink ref="J61" r:id="rId39" xr:uid="{B66CF1D7-6109-4F69-9E65-1E4FC473FAED}"/>
+    <hyperlink ref="J60" r:id="rId40" xr:uid="{CEE2AD88-0F61-4295-92F9-4954BBA23550}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId41"/>
   <tableParts count="1">
-    <tablePart r:id="rId34"/>
+    <tablePart r:id="rId42"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
updated control panel and moved seperating wall to avoid getting users stuck in it
</commit_message>
<xml_diff>
--- a/ResearchDiary/RelatedWorkTabelle.xlsx
+++ b/ResearchDiary/RelatedWorkTabelle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmaer\Documents\FH\Projects\MasterArbeit\mmt-masterarbeit-david-maerzendorfer\ResearchDiary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8FBC23-4CC2-44DF-B6E7-68AA12692B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA641011-A8D3-455E-A8E2-A20710E2C1BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="258">
   <si>
     <t>Paper</t>
   </si>
@@ -877,6 +877,18 @@
   </si>
   <si>
     <t>riku otono et al.</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/3613905.3650752</t>
+  </si>
+  <si>
+    <t>embodiment on hands in vr and stuff, interesting</t>
+  </si>
+  <si>
+    <t>Understanding the Impact of Coherence between Virtual Representations and Possible Interactions on Embodiment in VR: an Affordance Perspective</t>
+  </si>
+  <si>
+    <t>florian dufresne et al.</t>
   </si>
 </sst>
 </file>
@@ -1691,11 +1703,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L62" sqref="L62"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -2816,6 +2828,23 @@
       </c>
       <c r="J63" s="1" t="s">
         <v>250</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="180">
+      <c r="A64" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B64" s="30" t="s">
+        <v>256</v>
+      </c>
+      <c r="D64" s="1">
+        <v>2024</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="J64" s="7" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -2942,11 +2971,12 @@
     <hyperlink ref="J4" r:id="rId38" xr:uid="{1F3018DF-9A45-4184-8FF7-66A67C65CF9B}"/>
     <hyperlink ref="J61" r:id="rId39" xr:uid="{B66CF1D7-6109-4F69-9E65-1E4FC473FAED}"/>
     <hyperlink ref="J60" r:id="rId40" xr:uid="{CEE2AD88-0F61-4295-92F9-4954BBA23550}"/>
+    <hyperlink ref="J64" r:id="rId41" xr:uid="{D5C7C32A-84CC-4A29-945C-B18CC5904D11}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId41"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId42"/>
   <tableParts count="1">
-    <tablePart r:id="rId42"/>
+    <tablePart r:id="rId43"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
started with analysing the study result
</commit_message>
<xml_diff>
--- a/ResearchDiary/RelatedWorkTabelle.xlsx
+++ b/ResearchDiary/RelatedWorkTabelle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmaer\Documents\FH\Projects\MasterArbeit\mmt-masterarbeit-david-maerzendorfer\ResearchDiary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA641011-A8D3-455E-A8E2-A20710E2C1BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD13CE36-E29C-4B03-847A-7B7C0BC57712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="269">
   <si>
     <t>Paper</t>
   </si>
@@ -890,12 +890,66 @@
   <si>
     <t>florian dufresne et al.</t>
   </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S1053810005001200?via%3Dihub</t>
+  </si>
+  <si>
+    <t>body ownership</t>
+  </si>
+  <si>
+    <r>
+      <t>Having a body </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t>versus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t> moving your body: How agency structures body-ownership</t>
+    </r>
+  </si>
+  <si>
+    <t>manos tsakiris et al.</t>
+  </si>
+  <si>
+    <t>Neurofunctional correlates of body-ownership and sense of agency: A meta-analytical account of self-consciousness</t>
+  </si>
+  <si>
+    <t>giannini et al.</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0010945219303077#:~:text=Gallagher%20(2000)%20suggested%20that%20the,consequence%20(Gallagher%2C%202000).</t>
+  </si>
+  <si>
+    <t>Philosophical conceptions of the self: implications for cognitive science</t>
+  </si>
+  <si>
+    <t>gallagher et al.</t>
+  </si>
+  <si>
+    <t>og body ownership</t>
+  </si>
+  <si>
+    <t>https://www.cell.com/AJHG/fulltext/S1364-6613(99)01417-5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="30">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1088,6 +1142,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="16"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color rgb="FF2E2E2E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1140,7 +1213,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1233,6 +1306,12 @@
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1703,11 +1782,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K64"/>
+  <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J64" sqref="J64"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M66" sqref="M66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -2845,6 +2924,57 @@
       </c>
       <c r="J64" s="7" t="s">
         <v>254</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="40">
+      <c r="A65" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B65" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="D65" s="1">
+        <v>2006</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="60">
+      <c r="A66" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B66" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="D66" s="1">
+        <v>2019</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="82.5">
+      <c r="A67" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B67" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="D67" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated diary and added early version of latex code
</commit_message>
<xml_diff>
--- a/ResearchDiary/RelatedWorkTabelle.xlsx
+++ b/ResearchDiary/RelatedWorkTabelle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmaer\Documents\FH\Projects\MasterArbeit\mmt-masterarbeit-david-maerzendorfer\ResearchDiary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDC1C33-0382-452C-BE24-C3DE2B6F3B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC04C952-C3F6-442C-B42C-ED62F8CE436F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="304">
   <si>
     <t>Paper</t>
   </si>
@@ -1015,12 +1015,51 @@
   <si>
     <t>cao et al.</t>
   </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/3611659.3617219</t>
+  </si>
+  <si>
+    <t>drones in first person and how to make it more bearable</t>
+  </si>
+  <si>
+    <t>Sickness Reduction in FPV Drone Control: Improved Effects of Reverse Optical Flow with Static Landmarks Only</t>
+  </si>
+  <si>
+    <t>ryu et al.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2110.02514</t>
+  </si>
+  <si>
+    <t>using an extra panel/viewpoint for better selection of distant objects</t>
+  </si>
+  <si>
+    <t>ViewfinderVR: Configurable Viewfinder for Selection of Distant Objects in VR</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/221314246_Application_and_taxonomy_of_through-the-lens_techniques</t>
+  </si>
+  <si>
+    <t>through the lens method</t>
+  </si>
+  <si>
+    <t>Through-the-lens camera control</t>
+  </si>
+  <si>
+    <t>gleicher et al.</t>
+  </si>
+  <si>
+    <t>McCrae et al.</t>
+  </si>
+  <si>
+    <t>a better hoverCam interesting read, also stuff with up vector, is good for really big stuff, allows to scale it down and zoom in, eG whole earth modal and scale down to a house</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="36">
+  <fonts count="37">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1252,6 +1291,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="19.8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1304,7 +1350,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1412,6 +1458,9 @@
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1882,11 +1931,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K73"/>
+  <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A73" sqref="A73"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J72" sqref="J72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -3158,7 +3207,7 @@
       <c r="I72" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="J72" s="1" t="s">
+      <c r="J72" s="7" t="s">
         <v>283</v>
       </c>
     </row>
@@ -3177,6 +3226,74 @@
       </c>
       <c r="J73" s="1" t="s">
         <v>287</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="150">
+      <c r="A74" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B74" s="30" t="s">
+        <v>293</v>
+      </c>
+      <c r="D74" s="1">
+        <v>2023</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="75">
+      <c r="A75" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B75" s="38" t="s">
+        <v>297</v>
+      </c>
+      <c r="D75" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="J75" s="7" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="60">
+      <c r="A76" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B76" s="30" t="s">
+        <v>300</v>
+      </c>
+      <c r="D76" s="1">
+        <v>2002</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="43.5">
+      <c r="A77" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B77" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="D77" s="1">
+        <v>2009</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="J77" s="7" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -3308,11 +3425,14 @@
     <hyperlink ref="J23" r:id="rId43" xr:uid="{28435E4C-E883-4011-A9D5-6ED84832C910}"/>
     <hyperlink ref="J27" r:id="rId44" xr:uid="{388B35F5-691D-463F-B5E9-8D1A3D83D62C}"/>
     <hyperlink ref="J34" r:id="rId45" xr:uid="{550F363D-2754-4B47-A7B3-A05C83B85325}"/>
+    <hyperlink ref="J75" r:id="rId46" xr:uid="{F9D1EB43-A6DE-4003-814B-6211D96F629A}"/>
+    <hyperlink ref="J77" r:id="rId47" xr:uid="{2E14B2B9-BB74-4E4C-896C-00FF89B40DF7}"/>
+    <hyperlink ref="J72" r:id="rId48" xr:uid="{A8540BDA-151B-4DF1-9876-D1569544734C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId46"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId49"/>
   <tableParts count="1">
-    <tablePart r:id="rId47"/>
+    <tablePart r:id="rId50"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
removed old zed playground
</commit_message>
<xml_diff>
--- a/ResearchDiary/RelatedWorkTabelle.xlsx
+++ b/ResearchDiary/RelatedWorkTabelle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmaer\Documents\FH\Projects\MasterArbeit\mmt-masterarbeit-david-maerzendorfer\ResearchDiary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC04C952-C3F6-442C-B42C-ED62F8CE436F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE49082-DB74-4DE6-B58C-31C16197C545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1934,8 +1934,8 @@
   <dimension ref="A1:K77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J72" sqref="J72"/>
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J75" sqref="J75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -3037,7 +3037,7 @@
       <c r="I62" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="J62" s="1" t="s">
+      <c r="J62" s="7" t="s">
         <v>246</v>
       </c>
     </row>
@@ -3428,11 +3428,12 @@
     <hyperlink ref="J75" r:id="rId46" xr:uid="{F9D1EB43-A6DE-4003-814B-6211D96F629A}"/>
     <hyperlink ref="J77" r:id="rId47" xr:uid="{2E14B2B9-BB74-4E4C-896C-00FF89B40DF7}"/>
     <hyperlink ref="J72" r:id="rId48" xr:uid="{A8540BDA-151B-4DF1-9876-D1569544734C}"/>
+    <hyperlink ref="J62" r:id="rId49" xr:uid="{671E0915-5C51-437D-BF6E-163C52F69A68}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId49"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId50"/>
   <tableParts count="1">
-    <tablePart r:id="rId50"/>
+    <tablePart r:id="rId51"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>